<commit_message>
more small fixes for pivot
</commit_message>
<xml_diff>
--- a/tests/Templates/tPivot5_Static.xlsx
+++ b/tests/Templates/tPivot5_Static.xlsx
@@ -21,12 +21,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
   <si>
     <t>Static Pivot Table</t>
-  </si>
-  <si>
-    <t>delete</t>
   </si>
   <si>
     <t>Company</t>
@@ -105,21 +102,13 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="8"/>
       <color theme="1"/>
       <name val="Tahoma"/>
       <family val="2"/>
       <charset val="204"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="16"/>
-      <color indexed="9"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="16"/>
@@ -138,6 +127,28 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="16"/>
+      <color indexed="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -148,8 +159,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="54"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FF9F7CFF"/>
+        <bgColor indexed="42"/>
       </patternFill>
     </fill>
   </fills>
@@ -177,36 +188,36 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -223,6 +234,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -233,8 +246,10 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный 2" xfId="2"/>
+    <cellStyle name="Обычный 3" xfId="1"/>
   </cellStyles>
   <dxfs count="4">
     <dxf>
@@ -260,46 +275,39 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>590550</xdr:rowOff>
-    </xdr:to>
+    <xdr:ext cx="1695450" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 2" descr="I:\Images\4\bmpLogo4.gif"/>
+        <xdr:cNvPr id="3" name="Рисунок 2"/>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
-        <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
+      <xdr:spPr>
         <a:xfrm>
-          <a:off x="2352675" y="28575"/>
-          <a:ext cx="2238375" cy="561975"/>
+          <a:off x="2924175" y="0"/>
+          <a:ext cx="1695450" cy="609600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:noFill/>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
-  </xdr:twoCellAnchor>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -762,129 +770,129 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:8">
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
     </row>
     <row r="4" spans="2:8">
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
       <c r="E4" s="18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F4" s="20"/>
       <c r="G4" s="18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H4" s="18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="2:8">
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="D5" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="17" t="s">
-        <v>23</v>
+      <c r="E5" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>22</v>
       </c>
       <c r="G5" s="19"/>
       <c r="H5" s="19"/>
     </row>
     <row r="6" spans="2:8">
       <c r="B6" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="D6" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="12">
-        <v>0</v>
-      </c>
-      <c r="F6" s="12">
-        <v>0</v>
-      </c>
-      <c r="G6" s="12">
-        <v>0</v>
-      </c>
-      <c r="H6" s="13">
+      <c r="E6" s="10">
+        <v>0</v>
+      </c>
+      <c r="F6" s="10">
+        <v>0</v>
+      </c>
+      <c r="G6" s="10">
+        <v>0</v>
+      </c>
+      <c r="H6" s="11">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:8">
       <c r="B7" s="20"/>
       <c r="C7" s="18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D7" s="20"/>
-      <c r="E7" s="12">
-        <v>0</v>
-      </c>
-      <c r="F7" s="12">
-        <v>0</v>
-      </c>
-      <c r="G7" s="12">
-        <v>0</v>
-      </c>
-      <c r="H7" s="13">
+      <c r="E7" s="10">
+        <v>0</v>
+      </c>
+      <c r="F7" s="10">
+        <v>0</v>
+      </c>
+      <c r="G7" s="10">
+        <v>0</v>
+      </c>
+      <c r="H7" s="11">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:8">
       <c r="B8" s="18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" s="20"/>
       <c r="D8" s="20"/>
-      <c r="E8" s="12">
-        <v>0</v>
-      </c>
-      <c r="F8" s="12">
-        <v>0</v>
-      </c>
-      <c r="G8" s="12">
-        <v>0</v>
-      </c>
-      <c r="H8" s="13">
+      <c r="E8" s="10">
+        <v>0</v>
+      </c>
+      <c r="F8" s="10">
+        <v>0</v>
+      </c>
+      <c r="G8" s="10">
+        <v>0</v>
+      </c>
+      <c r="H8" s="11">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:8">
       <c r="B9" s="18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="20"/>
       <c r="D9" s="20"/>
-      <c r="E9" s="12">
-        <v>0</v>
-      </c>
-      <c r="F9" s="12">
-        <v>0</v>
-      </c>
-      <c r="G9" s="12">
-        <v>0</v>
-      </c>
-      <c r="H9" s="13">
+      <c r="E9" s="10">
+        <v>0</v>
+      </c>
+      <c r="F9" s="10">
+        <v>0</v>
+      </c>
+      <c r="G9" s="10">
+        <v>0</v>
+      </c>
+      <c r="H9" s="11">
         <v>0</v>
       </c>
     </row>
@@ -908,7 +916,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5"/>
@@ -918,78 +926,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="48" customHeight="1">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
+      <c r="B1" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
     </row>
     <row r="3" spans="1:8" ht="30.75" customHeight="1">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="19.5" customHeight="1">
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="D4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="F4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="G4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="H4" s="5" t="s">
         <v>14</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="11.25">
       <c r="A5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
+        <v>23</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C4">
@@ -998,6 +1001,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>